<commit_message>
Update dependencies and add document indexing notebook
- Changed the version of `azure-ai-translation-text` from `1.0.1` to `1.0.0b1` in `pyproject.toml` and `uv.lock`.
- Added a new Jupyter notebook `indexing_multilanguage.ipynb` demonstrating a structured document indexing workflow with language detection and translation.
- Created a new notebook `indexing_translate_english.ipynb` as a placeholder for future translation functionality.
</commit_message>
<xml_diff>
--- a/notebook/car_problems_multilingual.xlsx
+++ b/notebook/car_problems_multilingual.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,10 +451,15 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>ProblemType</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Fault</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Fix</t>
         </is>
@@ -463,88 +468,103 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>71dc2437-53c7-488a-90b2-cb01da2dfa21</t>
+          <t>4a0f47a5-2410-4bd6-8dc6-981027e592bc</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Accord</t>
+          <t>Passat</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Engine gets too hot</t>
+          <t>Surchauffe moteur</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Add coolant, inspect radiator for leaks</t>
+          <t>Problème de surchauffe moteur</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Verifier radiateur et liquide</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>15ec9cab-b104-4012-9a52-44062baa4722</t>
+          <t>a0a1ad1f-05e6-4f1e-bd2d-f380cf318eee</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Golf</t>
+          <t>Civic</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>Battery Drain</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>Battery draining fast</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>check alternator</t>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>new battery needed</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>a6cf70f7-07db-4a88-b27a-73080ad3fdc5</t>
+          <t>8da8e4a4-e217-411e-8c1e-7c4c768eeb83</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Nissan</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Camry</t>
+          <t>Altima</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ブレーキの音</t>
+          <t>Battery Drain</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>新しいブレーキパッド</t>
+          <t>Battery draining fast</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Test alternator and replace battery</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>49c3bcc3-8f13-4338-a5f4-c36310684ef2</t>
+          <t>e27c818e-df8d-4f70-8fd3-1064f9ae5142</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -554,159 +574,189 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Accord</t>
+          <t>Civic</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>battery dies quickly</t>
+          <t>Engine Overheating</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>new battery needed</t>
+          <t>overheating problem</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Add coolant, inspect radiator for leaks</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>0cb6b3b3-c5c0-4dd5-a9b0-b1905ad385c5</t>
+          <t>dc4bb767-f6ae-40ee-b89f-b0f5d50672d1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>פולקסווגן</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Sentra</t>
+          <t>גולף</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>刹车有噪音</t>
+          <t>ריקון סוללה</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>更换刹车片</t>
+          <t>הסוללה לא מחזיקה</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>החלף סוללה</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>b7c92f41-0a84-490f-8fdc-2abc1779a2a5</t>
+          <t>b58dc4c3-7e3e-4dfe-a993-5385809a8a29</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>Passat</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ブレーキノイズ</t>
+          <t>Engine Overheating</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>パッド替える</t>
+          <t>Engine gets too hot</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>coolant low - add more</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>fd4cdad6-ae02-4cee-bffe-3f465965aa84</t>
+          <t>69580655-2091-47ac-96c0-84c576a9d7a4</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>丰田</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Sentra</t>
+          <t>卡罗拉</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Engine overheating</t>
+          <t>刹车噪音</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Add coolant, inspect radiator for leaks</t>
+          <t>制动器噪音</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>更换刹车片</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>af206047-7371-40a5-a727-21be0f91a070</t>
+          <t>e7a13b1b-e06c-4014-b49e-5259ac8ccff3</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>Corolla</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Problème de surchauffe moteur</t>
+          <t>Battery Drain</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Vérifier niveau liquide refroidissement</t>
+          <t>battery dies quickly</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>new battery needed</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>9e56ad15-8ddb-4cb7-bc86-d31c6c0a2a85</t>
+          <t>f35a4427-a021-455a-b591-e44f660dbfdb</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>フォルクスワーゲン</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Accord</t>
+          <t>ゴルフ</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>le moteur chauffe trop</t>
+          <t>ブレーキノイズ</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Verifier radiateur et liquide</t>
+          <t>ブレーキがキーキー鳴る</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>パッド交換必要</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>09200892-00d1-4da2-b0b9-3d35943e6c43</t>
+          <t>18330958-10d9-4e6d-bcda-9aa3bbbad452</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -716,105 +766,125 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Golf</t>
+          <t>Passat</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>moteur trop chaud</t>
+          <t>Battery Drain</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Vérifier niveau liquide refroidissement</t>
+          <t>battery drain issue</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>new battery needed</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>acec8cdc-b1b0-4f8a-b609-d50eedb0d527</t>
+          <t>922022c4-8165-42c5-9fdd-a8bfb4ae6ea3</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Camry</t>
+          <t>Civic</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>battery dies quickly</t>
+          <t>Brake Noise</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>check alternator</t>
+          <t>ブレーキ音がする</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>パッド交換必要</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>e81915f5-80ec-4dbc-9316-7d70b4a084d9</t>
+          <t>13fbd2bc-1d03-4dba-9f66-e25718e16e19</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>大众</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Altima</t>
+          <t>帕萨特</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Engine overheating</t>
+          <t>刹车噪音</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>refill coolant and check radiator</t>
+          <t>制动器噪音</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>需要新刹车片</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>f7d8cdba-1c63-4716-9943-e3266ffab525</t>
+          <t>f20770ee-414c-4471-8979-b309de20ff16</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>フォルクスワーゲン</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Passat</t>
+          <t>パサート</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Problème de surchauffe moteur</t>
+          <t>ブレーキノイズ</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Vérifier niveau liquide refroidissement</t>
+          <t>ブレーキの音</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>新しいブレーキパッド</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ab852b7d-efcd-4473-aa52-9b59fb100aef</t>
+          <t>f4413e21-858c-4f37-8d98-1a3542cb4f3a</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -829,19 +899,24 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>ブレーキ音がする</t>
+          <t>Surchauffe moteur</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>パッド交換必要</t>
+          <t>le moteur chauffe trop</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>ajouter du liquide de refroidissement</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1b13084a-ac69-4372-878d-ccf9a32dfa45</t>
+          <t>e36161d8-9759-4b88-afd5-6c7de28e6f3c</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -856,262 +931,312 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>ブレーキノイズ</t>
+          <t>Engine Overheating</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>パッド交換必要</t>
+          <t>engine is overheating</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Add coolant, inspect radiator for leaks</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2a78e2ba-d99b-492d-9e55-084668beb437</t>
+          <t>5a6b23d4-3ce5-4395-b229-929a104e3882</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Camry</t>
+          <t>Civic</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>刹车响</t>
+          <t>Brake Noise</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>更换刹车片</t>
+          <t>刹车声音大</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>需要新刹车片</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>88e3aad7-decf-44fe-a107-1d14fa8c4f62</t>
+          <t>164e30aa-730a-4ad7-8c11-e9b2dcc06088</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Altima</t>
+          <t>Focus</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>ブレーキノイズ</t>
+          <t>Surchauffe moteur</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>新しいブレーキパッド</t>
+          <t>Problème de surchauffe moteur</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>ajouter du liquide de refroidissement</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>9476ae9d-5c5b-4910-80c4-5d0f3606b1a7</t>
+          <t>5094a618-2b1e-4fcc-b4f9-f9acbae75256</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Focus</t>
+          <t>Accord</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>battery dies quickly</t>
+          <t>Surchauffe moteur</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>check alternator</t>
+          <t>le moteur chauffe trop</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>remplir liquide refroidissement</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ab27da77-df27-4a88-878e-3cb98704c1e5</t>
+          <t>318311b9-a7a5-4019-9ae7-44b8d18bbca0</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Civic</t>
+          <t>Camry</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
+          <t>Engine Overheating</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
           <t>Engine overheating</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Check coolant level and radiator</t>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Add coolant, inspect radiator for leaks</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>a8ba6b83-02a2-471c-994c-191925513e65</t>
+          <t>dcd29e60-3bc4-4bc7-b4ac-b9021d18c446</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>פורד</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Focus</t>
+          <t>פוקוס</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Engine overheating</t>
+          <t>ריקון סוללה</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>refill coolant and check radiator</t>
+          <t>סוללה מתרוקנת מהר</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>החלף סוללה</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>6744db8d-9ca0-43f4-83ad-ea705d7f193c</t>
+          <t>c30a31b6-e71a-41fc-a561-6a36e0a71582</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Altima</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>刹车响</t>
+          <t>Battery Drain</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>更换刹车片</t>
+          <t>battery drain issue</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>check alternator</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>397981c5-3aa7-42f5-a3a8-eac4654bdf35</t>
+          <t>16bfec05-13a3-44f0-8462-815a744b43f2</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>福特</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Focus</t>
+          <t>福克斯</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Problème de surchauffe moteur</t>
+          <t>刹车噪音</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>ajouter du liquide de refroidissement</t>
+          <t>制动器噪音</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>换新刹车片</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>8d136819-bc32-4ec6-a843-566982fc5a39</t>
+          <t>d8bfaf80-e37c-4750-866d-be6ac5e5bdfa</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>הונדה</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Corolla</t>
+          <t>אקורד</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>刹车有噪音</t>
+          <t>ריקון סוללה</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>刹车片要换</t>
+          <t>הסוללה לא מחזיקה</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>צריך סוללה חדשה</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>bc5b4625-01bc-46bb-acd5-b000a8c69220</t>
+          <t>ef55621c-ccb9-4721-82b0-5f428aacbcc8</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>日产</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Civic</t>
+          <t>轩逸</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>moteur trop chaud</t>
+          <t>刹车噪音</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>ajouter du liquide de refroidissement</t>
+          <t>刹车声音大</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>需要新刹车片</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>8a42afba-ca63-4dbd-9a7e-611420172801</t>
+          <t>422446cb-b71f-4fe8-9351-9ba93f2de848</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1126,235 +1251,280 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>battery drain issue</t>
+          <t>Battery Drain</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>new battery needed</t>
+          <t>Battery draining fast</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Test alternator and replace battery</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>cbc7db70-75cd-4e0f-a205-8f738c020c1b</t>
+          <t>1762138f-d49a-4e82-ac96-850f79c3435d</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>大众</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Golf</t>
+          <t>高尔夫</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>הסוללה לא מחזיקה</t>
+          <t>刹车噪音</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>צריך סוללה חדשה</t>
+          <t>刹车响</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>换新刹车片</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1dbe9efb-bd1e-4e8b-a945-7c4cdfa88c69</t>
+          <t>3f40b9c5-02cd-4d3c-9f65-91b6fd4c4610</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Nissan</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Focus</t>
+          <t>Sentra</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>刹车响</t>
+          <t>Brake Noise</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>更换刹车片</t>
+          <t>ブレーキノイズ</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>新しいブレーキパッド</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>d61feade-5291-47b6-af84-606f084350c2</t>
+          <t>6c299251-da58-4ebd-8930-1c107e151fb6</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Nissan</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Accord</t>
+          <t>Sentra</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>ブレーキ音がする</t>
+          <t>Engine Overheating</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>パッド交換必要</t>
+          <t>overheating problem</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>coolant low - add more</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>f18a06e7-cac9-4184-80f2-37509668ef5d</t>
+          <t>8faf4f09-d655-410c-961b-ec1f72c52c7a</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>ホンダ</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Passat</t>
+          <t>アコード</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>刹车声音大</t>
+          <t>ブレーキノイズ</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>更换刹车片</t>
+          <t>ブレーキの音</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>パッド替える</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>095badfa-81d8-4f55-a658-53497de5d65a</t>
+          <t>2c654162-4028-43a2-b60b-10f7145435cb</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>טויוטה</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Civic</t>
+          <t>קאמרי</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>制动器噪音</t>
+          <t>ריקון סוללה</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>换新刹车片</t>
+          <t>סוללה נגמרת מהר</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>סוללה חדשה</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>6984effd-168d-4da8-995a-6bcbbb8e7ffb</t>
+          <t>1cd00868-1eec-4ede-a532-78ce9c691b1f</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Accord</t>
+          <t>Camry</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>刹车响</t>
+          <t>Brake Noise</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>更换刹车片</t>
+          <t>ブレーキの音</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>新しいブレーキパッド</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>823e5481-53a5-44d8-8f05-43e04c5235e5</t>
+          <t>549ee220-4ab6-4fd2-9414-de5f79debf08</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Altima</t>
+          <t>Passat</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>סוללה מתרוקנת מהר</t>
+          <t>Battery Drain</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>סוללה חדשה</t>
+          <t>בעיית סוללה</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>צריך סוללה חדשה</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ed0a57c6-5c58-46ce-84f6-466ecf5cf98d</t>
+          <t>0bdb1534-71c1-47b3-b9c8-e55ebac9db97</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>טויוטה</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>קורולה</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>סוללה נגמרת מהר</t>
+          <t>ריקון סוללה</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>בדוק אלטרנטור והחלף סוללה</t>
+          <t>סוללה מתרוקנת מהר</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>החלף סוללה</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2de239c1-5aa6-4cbe-adc6-98d37426f135</t>
+          <t>8762e26e-4160-4e34-87c2-7b7ff8c54511</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1369,181 +1539,216 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Moteur surchauffe</t>
+          <t>Brake Noise</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Verifier radiateur et liquide</t>
+          <t>刹车有噪音</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>更换刹车片</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>482eb636-3e72-4890-a3d6-3fef8371a6eb</t>
+          <t>da6390c5-cad2-474d-a33b-d1f1ca3a23eb</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Sentra</t>
+          <t>Camry</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Moteur surchauffe</t>
+          <t>Battery Drain</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>remplir liquide refroidissement</t>
+          <t>battery drain issue</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>check alternator</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>3ba32c42-28d2-4dec-b111-cc854bb0fe7e</t>
+          <t>3dc3f428-45cb-4a3b-9f29-dafeffdba924</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Golf</t>
+          <t>Corolla</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>刹车声音大</t>
+          <t>Brake Noise</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>需要新刹车片</t>
+          <t>ブレーキの音</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>新しいブレーキパッド</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>676c2f72-4d2b-435f-99b5-2ea1292708fa</t>
+          <t>8c96ef54-59f4-4898-8da6-63c56db5ab36</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>ניסאן</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>אלטימה</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Engine overheating</t>
+          <t>ריקון סוללה</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Add coolant, inspect radiator for leaks</t>
+          <t>סוללה נגמרת מהר</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>החלף סוללה</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>3cf494d2-288e-4caa-8041-6ac53552412c</t>
+          <t>7a3df4d7-ff72-49e3-8c2c-b6b70cf29b8c</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Altima</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Battery won't hold charge</t>
+          <t>Engine Overheating</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>new battery needed</t>
+          <t>overheating problem</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>refill coolant and check radiator</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>9933cbea-13e9-4887-b733-50c0f9bf0930</t>
+          <t>cfcab74b-7a36-4524-baf1-db01a06cfb28</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Focus</t>
+          <t>Golf</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>בעיית סוללה</t>
+          <t>Engine Overheating</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>סוללה חדשה</t>
+          <t>engine is overheating</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Check coolant level and radiator</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>bab2db02-99bd-4326-b021-48e807f77fd4</t>
+          <t>5262f946-a833-457e-8ac6-82f73425a79e</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>フォード</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Passat</t>
+          <t>フォーカス</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>סוללה נגמרת מהר</t>
+          <t>ブレーキノイズ</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>סוללה חדשה</t>
+          <t>ブレーキノイズ</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>パッド替える</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>35554ec8-b8a6-4dbe-8ccf-b81069759f42</t>
+          <t>36f21ee5-cb47-4e4c-8205-cd4e78c4b491</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1558,127 +1763,152 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Battery draining fast</t>
+          <t>Surchauffe moteur</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>new battery needed</t>
+          <t>Moteur surchauffe</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>remplir liquide refroidissement</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ffd74b37-b05d-44af-8fa8-3303662f069b</t>
+          <t>83a490c9-1c66-4c82-9467-efd5551101dc</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Nissan</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Corolla</t>
+          <t>Sentra</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
+          <t>Engine Overheating</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
           <t>Problème de surchauffe moteur</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Verifier radiateur et liquide</t>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Vérifier niveau liquide refroidissement</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6ab402b1-745f-4d4e-8aee-d396b0776d72</t>
+          <t>e4ca1d7a-501d-4bae-9a28-65bc07a73d89</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>הונדה</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Passat</t>
+          <t>סיוויק</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>engine is overheating</t>
+          <t>ריקון סוללה</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Check coolant level and radiator</t>
+          <t>סוללה נגמרת מהר</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>החלף סוללה</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>3fca2773-bed2-41e1-aab9-e382b743ebe8</t>
+          <t>c5327d3f-cd5e-4f9c-bac0-0e5c09f180b9</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Nissan</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Civic</t>
+          <t>Altima</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>סוללה נגמרת מהר</t>
+          <t>Brake Noise</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>סוללה חדשה</t>
+          <t>刹车声音大</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>更换刹车片</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>41f3e4d1-094b-456b-be12-de2bbadaec9a</t>
+          <t>e37d1cb9-fd0d-4103-bea3-b054ed4ebc9b</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Accord</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>סוללה מתרוקנת מהר</t>
+          <t>Surchauffe moteur</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>צריך סוללה חדשה</t>
+          <t>moteur trop chaud</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Vérifier niveau liquide refroidissement</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>bf39c622-2e1a-49cd-95b4-f2547d0ae061</t>
+          <t>6ae96a95-0d1a-49ad-83aa-30369eee762f</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1693,118 +1923,143 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>overheating problem</t>
+          <t>Engine Overheating</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>coolant low - add more</t>
+          <t>engine is overheating</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>refill coolant and check radiator</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>7ee6a48a-36c7-45ef-ad97-8ada2dae11e4</t>
+          <t>f1fa5373-f8b5-4a76-b41f-393737a5d2b5</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Nissan</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Passat</t>
+          <t>Altima</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>ブレーキ音がする</t>
+          <t>Engine Overheating</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>パッド替える</t>
+          <t>Engine overheating</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>coolant low - add more</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>c1e5c74a-cd44-4993-b197-a2290f8d7b9f</t>
+          <t>e6a5e1f3-0575-489c-a3bc-caac3c8976b8</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Camry</t>
+          <t>Accord</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>סוללה מתרוקנת מהר</t>
+          <t>Engine Overheating</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>החלף סוללה</t>
+          <t>overheating problem</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Check coolant level and radiator</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>7f6ab1c2-01d7-47c0-960a-ebfb6ee0ca65</t>
+          <t>d373132d-aabb-4949-ae82-b91cfba45465</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Corolla</t>
+          <t>Accord</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Battery won't hold charge</t>
+          <t>Battery Drain</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>check alternator</t>
+          <t>Battery draining fast</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>new battery needed</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>d73037fa-92a7-47bb-85f6-c23519eb6166</t>
+          <t>71fa1817-9f9b-4b69-b481-f4fccdaa9a20</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Civic</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
+          <t>Brake Noise</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
           <t>ブレーキがキーキー鳴る</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="F51" t="inlineStr">
         <is>
           <t>パッド替える</t>
         </is>
@@ -1813,34 +2068,39 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>4bf014b8-3a60-476a-bb30-e563e5227f05</t>
+          <t>9937c905-c854-45b5-b954-489ad3abd9ec</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Golf</t>
+          <t>Focus</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>ブレーキの音</t>
+          <t>Battery Drain</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>新しいブレーキパッド</t>
+          <t>battery dies quickly</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>new battery needed</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>1433b39f-37d4-48e8-a43b-d32863a2b3f7</t>
+          <t>5d9141d6-0321-45b4-be65-b611d05ebfc5</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1855,73 +2115,88 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>ブレーキ音がする</t>
+          <t>Battery Drain</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>パッド替える</t>
+          <t>סוללה מתרוקנת מהר</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>צריך סוללה חדשה</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>7034b553-3427-4fe3-b603-f764bfe506d2</t>
+          <t>b6549f2d-4eea-433f-a194-7ca10cf5b26b</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Nissan</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Golf</t>
+          <t>Altima</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>overheating problem</t>
+          <t>Surchauffe moteur</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>coolant low - add more</t>
+          <t>Moteur surchauffe</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Verifier radiateur et liquide</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>e8046a10-89fd-461c-a908-1f331f9dbc7b</t>
+          <t>37359cc0-69b5-4513-997c-a6b13375a8e0</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Camry</t>
+          <t>Golf</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Engine gets too hot</t>
+          <t>Surchauffe moteur</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Add coolant, inspect radiator for leaks</t>
+          <t>Moteur surchauffe</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Vérifier niveau liquide refroidissement</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>b4a423a8-797c-40b6-a24f-f16ec1d220b6</t>
+          <t>9dc96590-f0a1-442f-99ff-32decd3403d1</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1936,100 +2211,120 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>moteur trop chaud</t>
+          <t>Brake Noise</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Verifier radiateur et liquide</t>
+          <t>ブレーキの音</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>パッド交換必要</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>4fafb4fc-57dd-4c14-86bb-4c719510db26</t>
+          <t>dc9817c2-4152-41dc-abce-37bb442d073f</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Corolla</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>בעיית סוללה</t>
+          <t>Battery Drain</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>סוללה חדשה</t>
+          <t>סוללה מתרוקנת מהר</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>בדוק אלטרנטור והחלף סוללה</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>025d5ebb-3586-4323-8ee6-e3cd417256d5</t>
+          <t>3a6c8d1b-9a89-4fa1-a7a7-030967298c49</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>Accord</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>刹车响</t>
+          <t>Brake Noise</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>换新刹车片</t>
+          <t>制动器噪音</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>刹车片要换</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>47b835df-0c12-4186-8a1e-627baa0d2768</t>
+          <t>8ccfbf63-6cd9-4bef-b6b1-a5a3e6f56b08</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Sentra</t>
+          <t>Golf</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>הסוללה לא מחזיקה</t>
+          <t>Battery Drain</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>בדוק אלטרנטור והחלף סוללה</t>
+          <t>Battery draining fast</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Replace battery or alternator</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>7a58ea7a-5c48-4b3a-be4c-386c1531d3bf</t>
+          <t>f72e1002-14f8-4742-8239-8bf168b82df1</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2044,39 +2339,49 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Battery won't hold charge</t>
+          <t>Brake Noise</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>check alternator</t>
+          <t>刹车响</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>换新刹车片</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>b1c1a24b-a8a6-4446-9c18-d4fa661768cc</t>
+          <t>5108c6ee-6bab-4063-9a1b-34011ec0c3ff</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Passat</t>
+          <t>Camry</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>battery dies quickly</t>
+          <t>Engine Overheating</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Test alternator and replace battery</t>
+          <t>moteur trop chaud</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>ajouter du liquide de refroidissement</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor multilingual car problems dataset generation and indexing
- Removed problem type from dataset structure in `generate.data.ipynb`.
- Updated language mixing strategy descriptions for clarity.
- Adjusted execution counts and added necessary imports in `indexing_multilanguage.ipynb`.
- Enhanced comments and documentation for better understanding of language detection and embedding processes.
- Converted XLSX file to JSON format for easier processing.
- Fixed issues related to document properties in Azure search client.
</commit_message>
<xml_diff>
--- a/notebook/car_problems_multilingual.xlsx
+++ b/notebook/car_problems_multilingual.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,15 +451,10 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>ProblemType</t>
+          <t>Fault</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Fault</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Fix</t>
         </is>
@@ -468,382 +463,322 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>4a0f47a5-2410-4bd6-8dc6-981027e592bc</t>
+          <t>a4103b4e-38a2-4817-9394-18a52cd0bb06</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>丰田</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Passat</t>
+          <t>凯美瑞</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Surchauffe moteur</t>
+          <t>刹车有噪音</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Problème de surchauffe moteur</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Verifier radiateur et liquide</t>
+          <t>需要新刹车片</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>a0a1ad1f-05e6-4f1e-bd2d-f380cf318eee</t>
+          <t>22984e73-ad39-4b6f-b3ec-8f8400804a7d</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Civic</t>
+          <t>Golf</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Battery Drain</t>
+          <t>סוללה נגמרת מהר</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Battery draining fast</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>new battery needed</t>
+          <t>סוללה חדשה</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>8da8e4a4-e217-411e-8c1e-7c4c768eeb83</t>
+          <t>cc9871f0-1eb3-41d9-a29f-381be8b0ee1a</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Altima</t>
+          <t>Focus</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Battery Drain</t>
+          <t>ブレーキがキーキー鳴る</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Battery draining fast</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Test alternator and replace battery</t>
+          <t>パッド替える</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>e27c818e-df8d-4f70-8fd3-1064f9ae5142</t>
+          <t>addfc4c4-4497-42c6-8585-1aa8fb9926c7</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Nissan</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Civic</t>
+          <t>Sentra</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Engine Overheating</t>
+          <t>Battery won't hold charge</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>overheating problem</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Add coolant, inspect radiator for leaks</t>
+          <t>check alternator</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>dc4bb767-f6ae-40ee-b89f-b0f5d50672d1</t>
+          <t>03ccf10b-3491-4491-b432-f90868613e4a</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>פולקסווגן</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>גולף</t>
+          <t>Golf</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ריקון סוללה</t>
+          <t>engine is overheating</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>הסוללה לא מחזיקה</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>החלף סוללה</t>
+          <t>Check coolant level and radiator</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>b58dc4c3-7e3e-4dfe-a993-5385809a8a29</t>
+          <t>2b2d3a4c-a612-430d-ad46-710d51c58788</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Passat</t>
+          <t>Civic</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Engine Overheating</t>
+          <t>Engine overheating</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Engine gets too hot</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>coolant low - add more</t>
+          <t>Add coolant, inspect radiator for leaks</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>69580655-2091-47ac-96c0-84c576a9d7a4</t>
+          <t>fbb1ab9a-f57c-47f8-8028-7f40926d6693</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>丰田</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>卡罗拉</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>刹车噪音</t>
+          <t>ブレーキの音</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>制动器噪音</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>更换刹车片</t>
+          <t>パッド替える</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>e7a13b1b-e06c-4014-b49e-5259ac8ccff3</t>
+          <t>55e1af90-c49f-4a7a-a917-6c1a1506d19d</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>פולקסווגן</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Corolla</t>
+          <t>פאסאט</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Battery Drain</t>
+          <t>הסוללה לא מחזיקה</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>battery dies quickly</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>new battery needed</t>
+          <t>בדוק אלטרנטור והחלף סוללה</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>f35a4427-a021-455a-b591-e44f660dbfdb</t>
+          <t>cc9d2071-85d6-488a-906f-124188c15a69</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>フォルクスワーゲン</t>
+          <t>Nissan</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ゴルフ</t>
+          <t>Altima</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ブレーキノイズ</t>
+          <t>Moteur surchauffe</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ブレーキがキーキー鳴る</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>パッド交換必要</t>
+          <t>Vérifier niveau liquide refroidissement</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>18330958-10d9-4e6d-bcda-9aa3bbbad452</t>
+          <t>8236718b-ce57-4f03-a62d-fe32e51fff3f</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>フォルクスワーゲン</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Passat</t>
+          <t>パサート</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Battery Drain</t>
+          <t>ブレーキの音</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>battery drain issue</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>new battery needed</t>
+          <t>パッド交換必要</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>922022c4-8165-42c5-9fdd-a8bfb4ae6ea3</t>
+          <t>2b0db107-be46-4ab5-b4a3-239a9f764131</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Nissan</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Civic</t>
+          <t>Sentra</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Brake Noise</t>
+          <t>הסוללה לא מחזיקה</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>ブレーキ音がする</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>パッド交換必要</t>
+          <t>סוללה חדשה</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>13fbd2bc-1d03-4dba-9f66-e25718e16e19</t>
+          <t>a8deeed7-54c8-4b09-bc42-92423da39da1</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>大众</t>
+          <t>本田</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>帕萨特</t>
+          <t>雅阁</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>刹车噪音</t>
+          <t>刹车响</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
-        <is>
-          <t>制动器噪音</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
         <is>
           <t>需要新刹车片</t>
         </is>
@@ -852,39 +787,34 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>f20770ee-414c-4471-8979-b309de20ff16</t>
+          <t>61a962f5-31c9-4453-8752-9c31388c4f1c</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>フォルクスワーゲン</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>パサート</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>ブレーキノイズ</t>
+          <t>overheating problem</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>ブレーキの音</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>新しいブレーキパッド</t>
+          <t>refill coolant and check radiator</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>f4413e21-858c-4f37-8d98-1a3542cb4f3a</t>
+          <t>2b870455-0721-47ff-8393-48fc4e087195</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -899,88 +829,73 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Surchauffe moteur</t>
+          <t>engine is overheating</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>le moteur chauffe trop</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>ajouter du liquide de refroidissement</t>
+          <t>refill coolant and check radiator</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>e36161d8-9759-4b88-afd5-6c7de28e6f3c</t>
+          <t>599b964d-2752-4d3a-ad7b-444fd7de3b93</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Focus</t>
+          <t>Camry</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Engine Overheating</t>
+          <t>le moteur chauffe trop</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>engine is overheating</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Add coolant, inspect radiator for leaks</t>
+          <t>remplir liquide refroidissement</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>5a6b23d4-3ce5-4395-b229-929a104e3882</t>
+          <t>4cb1acf3-31a9-40d4-b1ac-bbf26f528d52</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>ניסאן</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Civic</t>
+          <t>אלטימה</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Brake Noise</t>
+          <t>סוללה מתרוקנת מהר</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>刹车声音大</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>需要新刹车片</t>
+          <t>בדוק אלטרנטור והחלף סוללה</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>164e30aa-730a-4ad7-8c11-e9b2dcc06088</t>
+          <t>1c470ca2-7224-4202-943d-262ac112b291</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -995,376 +910,316 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Surchauffe moteur</t>
+          <t>刹车声音大</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Problème de surchauffe moteur</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>ajouter du liquide de refroidissement</t>
+          <t>需要新刹车片</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5094a618-2b1e-4fcc-b4f9-f9acbae75256</t>
+          <t>932bb681-7951-4ee9-8c0b-b0a66b2a95c3</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Accord</t>
+          <t>Camry</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Surchauffe moteur</t>
+          <t>Battery won't hold charge</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>le moteur chauffe trop</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>remplir liquide refroidissement</t>
+          <t>Replace battery or alternator</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>318311b9-a7a5-4019-9ae7-44b8d18bbca0</t>
+          <t>6d2ecb0e-68ef-447e-a072-79b13d8daf20</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>טויוטה</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Camry</t>
+          <t>קאמרי</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Engine Overheating</t>
+          <t>סוללה מתרוקנת מהר</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Engine overheating</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Add coolant, inspect radiator for leaks</t>
+          <t>סוללה חדשה</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>dcd29e60-3bc4-4bc7-b4ac-b9021d18c446</t>
+          <t>e1e5d6a1-48f4-48f8-a2ac-64f3e62eb891</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>פורד</t>
+          <t>Nissan</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>פוקוס</t>
+          <t>Altima</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>ריקון סוללה</t>
+          <t>battery dies quickly</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>סוללה מתרוקנת מהר</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>החלף סוללה</t>
+          <t>check alternator</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>c30a31b6-e71a-41fc-a561-6a36e0a71582</t>
+          <t>ef458697-692a-4120-a9d7-275d89c0b478</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>Passat</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Battery Drain</t>
+          <t>制动器噪音</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>battery drain issue</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>check alternator</t>
+          <t>需要新刹车片</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>16bfec05-13a3-44f0-8462-815a744b43f2</t>
+          <t>36e08d61-5c81-440d-82fb-9ed0f9af1391</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>福特</t>
+          <t>Nissan</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>福克斯</t>
+          <t>Sentra</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>刹车噪音</t>
+          <t>ブレーキノイズ</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>制动器噪音</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>换新刹车片</t>
+          <t>パッド交換必要</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>d8bfaf80-e37c-4750-866d-be6ac5e5bdfa</t>
+          <t>6cbc6cab-1619-4d8a-8c6c-164d88e970ce</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>הונדה</t>
+          <t>Nissan</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>אקורד</t>
+          <t>Altima</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>ריקון סוללה</t>
+          <t>ブレーキ音がする</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>הסוללה לא מחזיקה</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>צריך סוללה חדשה</t>
+          <t>新しいブレーキパッド</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>ef55621c-ccb9-4721-82b0-5f428aacbcc8</t>
+          <t>d2140eac-eba5-4043-b022-a7b7bb465b17</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>日产</t>
+          <t>トヨタ</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>轩逸</t>
+          <t>カムリ</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>刹车噪音</t>
+          <t>ブレーキの音</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>刹车声音大</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>需要新刹车片</t>
+          <t>新しいブレーキパッド</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>422446cb-b71f-4fe8-9351-9ba93f2de848</t>
+          <t>97ccfa78-8439-4e1c-ab7d-90cf1e520d35</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>フォルクスワーゲン</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Sentra</t>
+          <t>ゴルフ</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Battery Drain</t>
+          <t>ブレーキの音</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Battery draining fast</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Test alternator and replace battery</t>
+          <t>ブレーキパッド交換</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1762138f-d49a-4e82-ac96-850f79c3435d</t>
+          <t>336941fc-24ea-475b-a59f-493cfd91b4df</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>大众</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>高尔夫</t>
+          <t>Accord</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>刹车噪音</t>
+          <t>Engine gets too hot</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>刹车响</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>换新刹车片</t>
+          <t>Add coolant, inspect radiator for leaks</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>3f40b9c5-02cd-4d3c-9f65-91b6fd4c4610</t>
+          <t>280363bd-a327-4962-abd9-202e01b68f9f</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>トヨタ</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Sentra</t>
+          <t>カローラ</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Brake Noise</t>
+          <t>ブレーキノイズ</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>ブレーキノイズ</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>新しいブレーキパッド</t>
+          <t>パッド交換必要</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>6c299251-da58-4ebd-8930-1c107e151fb6</t>
+          <t>5e679c85-e634-45d9-be5a-94f9d52d1f84</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>הונדה</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Sentra</t>
+          <t>אקורד</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Engine Overheating</t>
+          <t>סוללה נגמרת מהר</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>overheating problem</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>coolant low - add more</t>
+          <t>בדוק אלטרנטור והחלף סוללה</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>8faf4f09-d655-410c-961b-ec1f72c52c7a</t>
+          <t>bda90e0c-e712-492f-bb43-e69323b60da9</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1374,7 +1229,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>アコード</t>
+          <t>シビック</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1383,11 +1238,6 @@
         </is>
       </c>
       <c r="E30" t="inlineStr">
-        <is>
-          <t>ブレーキの音</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
         <is>
           <t>パッド替える</t>
         </is>
@@ -1396,39 +1246,34 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2c654162-4028-43a2-b60b-10f7145435cb</t>
+          <t>9592ca32-409b-4412-b351-439b78e8c37c</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>טויוטה</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>קאמרי</t>
+          <t>Passat</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>ריקון סוללה</t>
+          <t>Problème de surchauffe moteur</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>סוללה נגמרת מהר</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>סוללה חדשה</t>
+          <t>Vérifier niveau liquide refroidissement</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1cd00868-1eec-4ede-a532-78ce9c691b1f</t>
+          <t>b5d7be7f-50cf-4c87-ab9c-63281716434b</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1438,404 +1283,339 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Camry</t>
+          <t>Corolla</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Brake Noise</t>
+          <t>Battery draining fast</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>ブレーキの音</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>新しいブレーキパッド</t>
+          <t>Test alternator and replace battery</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>549ee220-4ab6-4fd2-9414-de5f79debf08</t>
+          <t>1b692d60-ce33-41ba-977d-209551ae13fe</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Passat</t>
+          <t>Corolla</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Battery Drain</t>
+          <t>Moteur surchauffe</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>בעיית סוללה</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>צריך סוללה חדשה</t>
+          <t>remplir liquide refroidissement</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>0bdb1534-71c1-47b3-b9c8-e55ebac9db97</t>
+          <t>920c8fe6-e698-46d4-9683-1ce9c189af41</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>טויוטה</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>קורולה</t>
+          <t>Focus</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>ריקון סוללה</t>
+          <t>overheating problem</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>סוללה מתרוקנת מהר</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>החלף סוללה</t>
+          <t>refill coolant and check radiator</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>8762e26e-4160-4e34-87c2-7b7ff8c54511</t>
+          <t>9a075ed3-1f28-4485-a1b7-e23598bcb04f</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Camry</t>
+          <t>Passat</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Brake Noise</t>
+          <t>battery dies quickly</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>刹车有噪音</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>更换刹车片</t>
+          <t>Replace battery or alternator</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>da6390c5-cad2-474d-a33b-d1f1ca3a23eb</t>
+          <t>4d73a2ca-0754-473f-ae8b-4fd2467e2d3c</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Camry</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Battery Drain</t>
+          <t>Moteur surchauffe</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>battery drain issue</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>check alternator</t>
+          <t>Verifier radiateur et liquide</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>3dc3f428-45cb-4a3b-9f29-dafeffdba924</t>
+          <t>3bc7d563-0412-4dfc-b263-8e35e6cfae33</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Corolla</t>
+          <t>Golf</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Brake Noise</t>
+          <t>刹车响</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>ブレーキの音</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>新しいブレーキパッド</t>
+          <t>更换刹车片</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>8c96ef54-59f4-4898-8da6-63c56db5ab36</t>
+          <t>2fd0b7ec-411a-4eff-862a-452b9193ffbd</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ניסאן</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>אלטימה</t>
+          <t>Accord</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>ריקון סוללה</t>
+          <t>Problème de surchauffe moteur</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>סוללה נגמרת מהר</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>החלף סוללה</t>
+          <t>Verifier radiateur et liquide</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>7a3df4d7-ff72-49e3-8c2c-b6b70cf29b8c</t>
+          <t>22d54f74-8504-49b4-9e3b-1af7e4790658</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Nissan</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>Altima</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Engine Overheating</t>
+          <t>刹车响</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>overheating problem</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>refill coolant and check radiator</t>
+          <t>需要新刹车片</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>cfcab74b-7a36-4524-baf1-db01a06cfb28</t>
+          <t>6232c9a2-ae99-4ed5-920d-49d3ca40d15b</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Nissan</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Golf</t>
+          <t>Sentra</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Engine Overheating</t>
+          <t>overheating problem</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>engine is overheating</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>Check coolant level and radiator</t>
+          <t>refill coolant and check radiator</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5262f946-a833-457e-8ac6-82f73425a79e</t>
+          <t>25c44b5f-3e5b-436b-a77e-686a1a535bd0</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>フォード</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>フォーカス</t>
+          <t>Accord</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>ブレーキノイズ</t>
+          <t>ブレーキ音がする</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>ブレーキノイズ</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>パッド替える</t>
+          <t>新しいブレーキパッド</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>36f21ee5-cb47-4e4c-8205-cd4e78c4b491</t>
+          <t>c2da9987-cc8b-401a-aac0-f71b20e649da</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Nissan</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Civic</t>
+          <t>Sentra</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Surchauffe moteur</t>
+          <t>moteur trop chaud</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Moteur surchauffe</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>remplir liquide refroidissement</t>
+          <t>ajouter du liquide de refroidissement</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>83a490c9-1c66-4c82-9467-efd5551101dc</t>
+          <t>dfd8c456-1c25-4b3e-a7dc-9c15c501223c</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Sentra</t>
+          <t>Camry</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Engine Overheating</t>
+          <t>Engine gets too hot</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Problème de surchauffe moteur</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>Vérifier niveau liquide refroidissement</t>
+          <t>Check coolant level and radiator</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>e4ca1d7a-501d-4bae-9a28-65bc07a73d89</t>
+          <t>8fc30268-c89f-4119-92d0-ff21fe6c7d7f</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>הונדה</t>
+          <t>טויוטה</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>סיוויק</t>
+          <t>קורולה</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>ריקון סוללה</t>
+          <t>סוללה נגמרת מהר</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
-        <is>
-          <t>סוללה נגמרת מהר</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
         <is>
           <t>החלף סוללה</t>
         </is>
@@ -1844,7 +1624,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>c5327d3f-cd5e-4f9c-bac0-0e5c09f180b9</t>
+          <t>913c99fb-e31d-4e69-be65-8c96932c5239</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1859,399 +1639,334 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Brake Noise</t>
+          <t>overheating problem</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>刹车声音大</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>更换刹车片</t>
+          <t>Add coolant, inspect radiator for leaks</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>e37d1cb9-fd0d-4103-bea3-b054ed4ebc9b</t>
+          <t>a555bd12-b5a9-458b-ae40-83836394b969</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>פורד</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>פוקוס</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Surchauffe moteur</t>
+          <t>סוללה מתרוקנת מהר</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>moteur trop chaud</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>Vérifier niveau liquide refroidissement</t>
+          <t>צריך סוללה חדשה</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6ae96a95-0d1a-49ad-83aa-30369eee762f</t>
+          <t>47758bb9-1549-4692-868b-9a6d1dfd355c</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Corolla</t>
+          <t>Golf</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Engine Overheating</t>
+          <t>Problème de surchauffe moteur</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>engine is overheating</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>refill coolant and check radiator</t>
+          <t>remplir liquide refroidissement</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>f1fa5373-f8b5-4a76-b41f-393737a5d2b5</t>
+          <t>191a721b-ab15-4033-93aa-a77f14fe5783</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>本田</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Altima</t>
+          <t>思域</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Engine Overheating</t>
+          <t>制动器噪音</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Engine overheating</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>coolant low - add more</t>
+          <t>更换刹车片</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>e6a5e1f3-0575-489c-a3bc-caac3c8976b8</t>
+          <t>ac470cdf-6de1-4936-85ff-5a3e3922f955</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Accord</t>
+          <t>Focus</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Engine Overheating</t>
+          <t>Problème de surchauffe moteur</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>overheating problem</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>Check coolant level and radiator</t>
+          <t>Verifier radiateur et liquide</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>d373132d-aabb-4949-ae82-b91cfba45465</t>
+          <t>9751150a-b44e-45cb-a4c1-6af8672597ad</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>הונדה</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Accord</t>
+          <t>סיוויק</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Battery Drain</t>
+          <t>בעיית סוללה</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Battery draining fast</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>new battery needed</t>
+          <t>בדוק אלטרנטור והחלף סוללה</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>71fa1817-9f9b-4b69-b481-f4fccdaa9a20</t>
+          <t>0fb94acd-af96-4386-aaab-d29275de1b92</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>福特</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>蒙迪欧</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Brake Noise</t>
+          <t>刹车有噪音</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>ブレーキがキーキー鳴る</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>パッド替える</t>
+          <t>换新刹车片</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>9937c905-c854-45b5-b954-489ad3abd9ec</t>
+          <t>d7ceac0d-6da1-4b2c-8df3-e6b164ab35ba</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Focus</t>
+          <t>Civic</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Battery Drain</t>
+          <t>le moteur chauffe trop</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>battery dies quickly</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>new battery needed</t>
+          <t>Verifier radiateur et liquide</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>5d9141d6-0321-45b4-be65-b611d05ebfc5</t>
+          <t>a005b016-257e-47ea-8c02-93d2e9e18606</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Sentra</t>
+          <t>Accord</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Battery Drain</t>
+          <t>Battery draining fast</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>סוללה מתרוקנת מהר</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>צריך סוללה חדשה</t>
+          <t>check alternator</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>b6549f2d-4eea-433f-a194-7ca10cf5b26b</t>
+          <t>bec9b183-e5d7-49bc-98c5-1c41b0c62993</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Altima</t>
+          <t>Focus</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Surchauffe moteur</t>
+          <t>Battery draining fast</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Moteur surchauffe</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>Verifier radiateur et liquide</t>
+          <t>Replace battery or alternator</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>37359cc0-69b5-4513-997c-a6b13375a8e0</t>
+          <t>68ca74ed-735d-47ee-9551-94bc29f0b2d0</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Golf</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Surchauffe moteur</t>
+          <t>battery drain issue</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Moteur surchauffe</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>Vérifier niveau liquide refroidissement</t>
+          <t>Test alternator and replace battery</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>9dc96590-f0a1-442f-99ff-32decd3403d1</t>
+          <t>49fd570e-20c7-4ff1-9ed5-6b65a1b77765</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Nissan</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Altima</t>
+          <t>Golf</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Brake Noise</t>
+          <t>Battery won't hold charge</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>ブレーキの音</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>パッド交換必要</t>
+          <t>Replace battery or alternator</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>dc9817c2-4152-41dc-abce-37bb442d073f</t>
+          <t>b55da832-0b7b-4e07-b60b-5878f3a8f549</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>פורד</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>פיוז'ן</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Battery Drain</t>
+          <t>סוללה מתרוקנת מהר</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
-        <is>
-          <t>סוללה מתרוקנת מהר</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
         <is>
           <t>בדוק אלטרנטור והחלף סוללה</t>
         </is>
@@ -2260,128 +1975,108 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>3a6c8d1b-9a89-4fa1-a7a7-030967298c49</t>
+          <t>e5063b51-0ef9-4e26-9680-d5f3bb4862e5</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>丰田</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Accord</t>
+          <t>卡罗拉</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Brake Noise</t>
+          <t>刹车声音大</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>制动器噪音</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>刹车片要换</t>
+          <t>需要新刹车片</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>8ccfbf63-6cd9-4bef-b6b1-a5a3e6f56b08</t>
+          <t>1beb9597-ac69-4a24-a822-6c6f42f7ff25</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Golf</t>
+          <t>Civic</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Battery Drain</t>
+          <t>battery drain issue</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Battery draining fast</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>Replace battery or alternator</t>
+          <t>new battery needed</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>f72e1002-14f8-4742-8239-8bf168b82df1</t>
+          <t>224a980a-2d2f-426a-8464-94d093b447ee</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>Passat</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Brake Noise</t>
+          <t>Engine overheating</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>刹车响</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>换新刹车片</t>
+          <t>refill coolant and check radiator</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>5108c6ee-6bab-4063-9a1b-34011ec0c3ff</t>
+          <t>74c67b8b-2637-4c04-acfb-2cf4b9d65a69</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>日产</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Camry</t>
+          <t>轩逸</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Engine Overheating</t>
+          <t>刹车有噪音</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>moteur trop chaud</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>ajouter du liquide de refroidissement</t>
+          <t>更换刹车片</t>
         </is>
       </c>
     </row>

</xml_diff>